<commit_message>
annotated schematic with necessary changes to load cell circuit. added pull-ups for enable PMOSes
</commit_message>
<xml_diff>
--- a/Nestbox_v2/BOM_Nestbox_v2.xlsx
+++ b/Nestbox_v2/BOM_Nestbox_v2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23580" windowHeight="20540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="3000" windowWidth="30160" windowHeight="23540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="BOM_Nestbox_v2.csv" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="230">
   <si>
     <t>Source:</t>
   </si>
@@ -405,18 +405,12 @@
     <t>R201</t>
   </si>
   <si>
-    <t>100k</t>
-  </si>
-  <si>
     <t>device:R</t>
   </si>
   <si>
     <t>Resistors_SMD:R_0603</t>
   </si>
   <si>
-    <t>50k</t>
-  </si>
-  <si>
     <t>R203</t>
   </si>
   <si>
@@ -426,15 +420,9 @@
     <t>R204</t>
   </si>
   <si>
-    <t>162k</t>
-  </si>
-  <si>
     <t>R205</t>
   </si>
   <si>
-    <t>649k</t>
-  </si>
-  <si>
     <t>R206</t>
   </si>
   <si>
@@ -465,9 +453,6 @@
     <t>DNP</t>
   </si>
   <si>
-    <t>1k 1%</t>
-  </si>
-  <si>
     <t>100R 1%</t>
   </si>
   <si>
@@ -480,12 +465,6 @@
     <t>2k2</t>
   </si>
   <si>
-    <t>18k</t>
-  </si>
-  <si>
-    <t>33k</t>
-  </si>
-  <si>
     <t>SW301</t>
   </si>
   <si>
@@ -667,6 +646,69 @@
   </si>
   <si>
     <t>SDSDQAB-008G</t>
+  </si>
+  <si>
+    <t>NOTES</t>
+  </si>
+  <si>
+    <t>Change to 805 size</t>
+  </si>
+  <si>
+    <t>rename</t>
+  </si>
+  <si>
+    <t>change footprint and/or value. Placed 10 uf</t>
+  </si>
+  <si>
+    <t>rename; wrong MPN, is not in würth box. Used 24pf</t>
+  </si>
+  <si>
+    <t>check land pattern with datasheet</t>
+  </si>
+  <si>
+    <t>silkscreen illegible</t>
+  </si>
+  <si>
+    <t>consolidate with other inductor possible?</t>
+  </si>
+  <si>
+    <t>??? Are the component names inverted???</t>
+  </si>
+  <si>
+    <t>consolidate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">consolidate </t>
+  </si>
+  <si>
+    <t>82k 1%</t>
+  </si>
+  <si>
+    <t>47K 1%</t>
+  </si>
+  <si>
+    <t>R701 could be 82k</t>
+  </si>
+  <si>
+    <t>rename --&gt; 10k</t>
+  </si>
+  <si>
+    <t>1k 0.1%</t>
+  </si>
+  <si>
+    <t>162k 1%</t>
+  </si>
+  <si>
+    <t>649k 1%</t>
+  </si>
+  <si>
+    <t>C602 label confusing position</t>
+  </si>
+  <si>
+    <t>could maybe be consolidated with LED resistor values</t>
+  </si>
+  <si>
+    <t>inductor too close.. Pads of tps not accessible</t>
   </si>
 </sst>
 </file>
@@ -713,7 +755,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -744,6 +786,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -754,7 +802,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="16">
+  <cellStyleXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -771,8 +819,18 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -782,8 +840,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="16">
+  <cellStyles count="26">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -793,12 +852,22 @@
     <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="21" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="23" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="25" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="16" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="18" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="20" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="22" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="24" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1128,19 +1197,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L73"/>
+  <dimension ref="A1:M73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="J73" sqref="J73"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="3" max="3" width="30.1640625" customWidth="1"/>
+    <col min="3" max="3" width="44" customWidth="1"/>
     <col min="4" max="4" width="23.6640625" customWidth="1"/>
+    <col min="13" max="13" width="10.83203125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:13">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1148,7 +1218,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:13">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1156,7 +1226,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:13">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1164,7 +1234,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:13">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1172,7 +1242,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:13">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1180,7 +1250,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:13">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -1217,16 +1287,19 @@
       <c r="L7" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="8" spans="1:12">
+      <c r="M7" s="6" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
       <c r="A8">
         <v>1</v>
       </c>
       <c r="B8">
         <v>7</v>
       </c>
-      <c r="C8" t="s">
-        <v>190</v>
+      <c r="C8" s="7" t="s">
+        <v>183</v>
       </c>
       <c r="D8" t="s">
         <v>21</v>
@@ -1237,16 +1310,19 @@
       <c r="F8" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="9" spans="1:12">
+      <c r="M8" s="6" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
       <c r="A9">
         <v>2</v>
       </c>
       <c r="B9">
         <v>5</v>
       </c>
-      <c r="C9" t="s">
-        <v>191</v>
+      <c r="C9" s="7" t="s">
+        <v>184</v>
       </c>
       <c r="D9" t="s">
         <v>24</v>
@@ -1258,14 +1334,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:13">
       <c r="A10">
         <v>3</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="7" t="s">
         <v>25</v>
       </c>
       <c r="D10" t="s">
@@ -1278,14 +1354,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:13">
       <c r="A11">
         <v>4</v>
       </c>
       <c r="B11">
         <v>1</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="7" t="s">
         <v>27</v>
       </c>
       <c r="D11" t="s">
@@ -1298,14 +1374,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:13">
       <c r="A12">
         <v>5</v>
       </c>
       <c r="B12">
         <v>1</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="7" t="s">
         <v>29</v>
       </c>
       <c r="D12" t="s">
@@ -1318,15 +1394,15 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:13">
       <c r="A13">
         <v>6</v>
       </c>
       <c r="B13">
         <v>4</v>
       </c>
-      <c r="C13" t="s">
-        <v>192</v>
+      <c r="C13" s="7" t="s">
+        <v>185</v>
       </c>
       <c r="D13" t="s">
         <v>31</v>
@@ -1338,15 +1414,15 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:13">
       <c r="A14">
         <v>7</v>
       </c>
       <c r="B14">
         <v>2</v>
       </c>
-      <c r="C14" t="s">
-        <v>193</v>
+      <c r="C14" s="7" t="s">
+        <v>186</v>
       </c>
       <c r="D14" t="s">
         <v>32</v>
@@ -1363,15 +1439,18 @@
       <c r="L14">
         <v>302010067</v>
       </c>
-    </row>
-    <row r="15" spans="1:12">
+      <c r="M14" s="6" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
       <c r="A15">
         <v>8</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="7" t="s">
         <v>35</v>
       </c>
       <c r="D15" t="s">
@@ -1386,15 +1465,18 @@
       <c r="K15" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="16" spans="1:12">
+      <c r="M15" s="6" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
       <c r="A16">
         <v>9</v>
       </c>
       <c r="B16">
         <v>1</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="7" t="s">
         <v>39</v>
       </c>
       <c r="D16" t="s">
@@ -1406,16 +1488,19 @@
       <c r="F16" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="17" spans="1:12">
+      <c r="M16" s="6" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13">
       <c r="A17">
         <v>10</v>
       </c>
       <c r="B17">
         <v>3</v>
       </c>
-      <c r="C17" t="s">
-        <v>194</v>
+      <c r="C17" s="7" t="s">
+        <v>187</v>
       </c>
       <c r="D17" t="s">
         <v>41</v>
@@ -1426,16 +1511,19 @@
       <c r="F17" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="18" spans="1:12">
+      <c r="M17" s="6" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13">
       <c r="A18" s="1">
         <v>11</v>
       </c>
       <c r="B18">
         <v>2</v>
       </c>
-      <c r="C18" t="s">
-        <v>195</v>
+      <c r="C18" s="7" t="s">
+        <v>188</v>
       </c>
       <c r="D18" t="s">
         <v>42</v>
@@ -1446,15 +1534,18 @@
       <c r="F18" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="19" spans="1:12">
+      <c r="M18" s="6" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13">
       <c r="A19">
         <v>12</v>
       </c>
       <c r="B19">
         <v>1</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="7" t="s">
         <v>45</v>
       </c>
       <c r="D19" t="s">
@@ -1466,8 +1557,11 @@
       <c r="F19" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="20" spans="1:12">
+      <c r="M19" s="6" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13">
       <c r="A20" s="1">
         <v>13</v>
       </c>
@@ -1487,7 +1581,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:12">
+    <row r="21" spans="1:13">
       <c r="A21" s="1">
         <v>14</v>
       </c>
@@ -1498,7 +1592,7 @@
         <v>51</v>
       </c>
       <c r="D21" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="E21" t="s">
         <v>52</v>
@@ -1513,7 +1607,7 @@
         <v>304090043</v>
       </c>
     </row>
-    <row r="22" spans="1:12">
+    <row r="22" spans="1:13">
       <c r="A22">
         <v>15</v>
       </c>
@@ -1539,7 +1633,7 @@
         <v>304090045</v>
       </c>
     </row>
-    <row r="23" spans="1:12">
+    <row r="23" spans="1:13">
       <c r="A23">
         <v>16</v>
       </c>
@@ -1559,7 +1653,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="24" spans="1:12">
+    <row r="24" spans="1:13">
       <c r="A24">
         <v>17</v>
       </c>
@@ -1579,7 +1673,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="25" spans="1:12">
+    <row r="25" spans="1:13">
       <c r="A25">
         <v>18</v>
       </c>
@@ -1599,7 +1693,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="26" spans="1:12">
+    <row r="26" spans="1:13">
       <c r="A26">
         <v>19</v>
       </c>
@@ -1619,7 +1713,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="27" spans="1:12">
+    <row r="27" spans="1:13">
       <c r="A27">
         <v>20</v>
       </c>
@@ -1639,7 +1733,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="28" spans="1:12">
+    <row r="28" spans="1:13">
       <c r="A28">
         <v>21</v>
       </c>
@@ -1659,7 +1753,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="29" spans="1:12">
+    <row r="29" spans="1:13">
       <c r="A29">
         <v>22</v>
       </c>
@@ -1679,7 +1773,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="30" spans="1:12">
+    <row r="30" spans="1:13">
       <c r="A30">
         <v>23</v>
       </c>
@@ -1699,7 +1793,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="31" spans="1:12">
+    <row r="31" spans="1:13">
       <c r="A31">
         <v>24</v>
       </c>
@@ -1719,7 +1813,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="32" spans="1:12">
+    <row r="32" spans="1:13">
       <c r="A32">
         <v>25</v>
       </c>
@@ -1739,7 +1833,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="33" spans="1:12">
+    <row r="33" spans="1:13">
       <c r="A33">
         <v>26</v>
       </c>
@@ -1759,14 +1853,14 @@
         <v>96</v>
       </c>
     </row>
-    <row r="34" spans="1:12">
+    <row r="34" spans="1:13">
       <c r="A34" s="2">
         <v>27</v>
       </c>
       <c r="B34">
         <v>1</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" s="7" t="s">
         <v>97</v>
       </c>
       <c r="D34" t="s">
@@ -1781,15 +1875,18 @@
       <c r="H34" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="35" spans="1:12">
+      <c r="M34" s="6" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13">
       <c r="A35" s="2">
         <v>28</v>
       </c>
       <c r="B35">
         <v>1</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C35" s="7" t="s">
         <v>102</v>
       </c>
       <c r="D35" t="s">
@@ -1804,15 +1901,18 @@
       <c r="I35" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="36" spans="1:12">
+      <c r="M35" s="6" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13">
       <c r="A36">
         <v>29</v>
       </c>
       <c r="B36">
         <v>1</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C36" s="7" t="s">
         <v>106</v>
       </c>
       <c r="D36" t="s">
@@ -1828,7 +1928,7 @@
         <v>303030020</v>
       </c>
     </row>
-    <row r="37" spans="1:12">
+    <row r="37" spans="1:13">
       <c r="A37">
         <v>30</v>
       </c>
@@ -1848,7 +1948,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="38" spans="1:12">
+    <row r="38" spans="1:13">
       <c r="A38">
         <v>31</v>
       </c>
@@ -1868,7 +1968,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="39" spans="1:12">
+    <row r="39" spans="1:13">
       <c r="A39">
         <v>32</v>
       </c>
@@ -1888,18 +1988,18 @@
         <v>112</v>
       </c>
     </row>
-    <row r="40" spans="1:12">
+    <row r="40" spans="1:13">
       <c r="A40" s="3">
         <v>33</v>
       </c>
       <c r="B40">
         <v>1</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C40" s="7" t="s">
         <v>117</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="E40" t="s">
         <v>118</v>
@@ -1908,15 +2008,15 @@
         <v>119</v>
       </c>
     </row>
-    <row r="41" spans="1:12">
+    <row r="41" spans="1:13">
       <c r="A41" s="3">
         <v>34</v>
       </c>
       <c r="B41">
         <v>2</v>
       </c>
-      <c r="C41" t="s">
-        <v>196</v>
+      <c r="C41" s="7" t="s">
+        <v>189</v>
       </c>
       <c r="D41" t="s">
         <v>120</v>
@@ -1928,15 +2028,15 @@
         <v>122</v>
       </c>
     </row>
-    <row r="42" spans="1:12">
+    <row r="42" spans="1:13">
       <c r="A42" s="3">
         <v>35</v>
       </c>
       <c r="B42">
         <v>2</v>
       </c>
-      <c r="C42" t="s">
-        <v>197</v>
+      <c r="C42" s="7" t="s">
+        <v>190</v>
       </c>
       <c r="D42" t="s">
         <v>123</v>
@@ -1948,15 +2048,15 @@
         <v>122</v>
       </c>
     </row>
-    <row r="43" spans="1:12">
+    <row r="43" spans="1:13">
       <c r="A43" s="1">
         <v>36</v>
       </c>
       <c r="B43">
         <v>2</v>
       </c>
-      <c r="C43" t="s">
-        <v>198</v>
+      <c r="C43" s="7" t="s">
+        <v>191</v>
       </c>
       <c r="D43" t="s">
         <v>124</v>
@@ -1968,14 +2068,14 @@
         <v>122</v>
       </c>
     </row>
-    <row r="44" spans="1:12">
+    <row r="44" spans="1:13">
       <c r="A44" s="3">
         <v>37</v>
       </c>
       <c r="B44">
         <v>1</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C44" s="7" t="s">
         <v>126</v>
       </c>
       <c r="D44" s="6" t="s">
@@ -1988,359 +2088,374 @@
         <v>122</v>
       </c>
     </row>
-    <row r="45" spans="1:12">
+    <row r="45" spans="1:13">
       <c r="A45">
         <v>38</v>
       </c>
       <c r="B45">
         <v>1</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C45" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="D45" t="s">
+      <c r="D45" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="E45" t="s">
         <v>128</v>
       </c>
-      <c r="E45" t="s">
+      <c r="F45" t="s">
         <v>129</v>
       </c>
-      <c r="F45" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12">
+      <c r="M45" s="6" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13">
       <c r="A46">
         <v>39</v>
       </c>
       <c r="B46">
         <v>2</v>
       </c>
-      <c r="C46" t="s">
-        <v>199</v>
-      </c>
-      <c r="D46" t="s">
-        <v>131</v>
+      <c r="C46" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="D46" s="6" t="s">
+        <v>221</v>
       </c>
       <c r="E46" t="s">
+        <v>128</v>
+      </c>
+      <c r="F46" t="s">
         <v>129</v>
       </c>
-      <c r="F46" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12">
+      <c r="M46" s="6" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13">
       <c r="A47">
         <v>40</v>
       </c>
       <c r="B47">
         <v>1</v>
       </c>
-      <c r="C47" t="s">
-        <v>132</v>
+      <c r="C47" s="7" t="s">
+        <v>130</v>
       </c>
       <c r="D47" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E47" t="s">
+        <v>128</v>
+      </c>
+      <c r="F47" t="s">
         <v>129</v>
       </c>
-      <c r="F47" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12">
+    </row>
+    <row r="48" spans="1:13">
       <c r="A48" s="3">
         <v>41</v>
       </c>
       <c r="B48">
         <v>1</v>
       </c>
-      <c r="C48" t="s">
-        <v>134</v>
-      </c>
-      <c r="D48" t="s">
-        <v>135</v>
+      <c r="C48" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="D48" s="6" t="s">
+        <v>225</v>
       </c>
       <c r="E48" t="s">
+        <v>128</v>
+      </c>
+      <c r="F48" t="s">
         <v>129</v>
       </c>
-      <c r="F48" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="49" spans="1:12">
+    </row>
+    <row r="49" spans="1:13">
       <c r="A49" s="3">
         <v>42</v>
       </c>
       <c r="B49">
         <v>1</v>
       </c>
-      <c r="C49" t="s">
-        <v>136</v>
-      </c>
-      <c r="D49" t="s">
-        <v>137</v>
+      <c r="C49" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="D49" s="6" t="s">
+        <v>226</v>
       </c>
       <c r="E49" t="s">
+        <v>128</v>
+      </c>
+      <c r="F49" t="s">
         <v>129</v>
       </c>
-      <c r="F49" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="50" spans="1:12">
+    </row>
+    <row r="50" spans="1:13">
       <c r="A50">
         <v>43</v>
       </c>
       <c r="B50">
         <v>1</v>
       </c>
-      <c r="C50" t="s">
-        <v>138</v>
+      <c r="C50" s="7" t="s">
+        <v>134</v>
       </c>
       <c r="D50" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E50" t="s">
+        <v>128</v>
+      </c>
+      <c r="F50" t="s">
         <v>129</v>
       </c>
-      <c r="F50" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="51" spans="1:12">
+    </row>
+    <row r="51" spans="1:13">
       <c r="A51">
         <v>44</v>
       </c>
       <c r="B51">
         <v>1</v>
       </c>
-      <c r="C51" t="s">
-        <v>140</v>
+      <c r="C51" s="7" t="s">
+        <v>136</v>
       </c>
       <c r="D51" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="E51" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="F51" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J51" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="L51">
         <v>301020022</v>
       </c>
-    </row>
-    <row r="52" spans="1:12">
+      <c r="M51" s="6" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13">
       <c r="A52">
         <v>45</v>
       </c>
       <c r="B52">
         <v>6</v>
       </c>
-      <c r="C52" t="s">
-        <v>200</v>
+      <c r="C52" s="7" t="s">
+        <v>193</v>
       </c>
       <c r="D52" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="E52" t="s">
+        <v>128</v>
+      </c>
+      <c r="F52" t="s">
         <v>129</v>
       </c>
-      <c r="F52" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="53" spans="1:12">
+    </row>
+    <row r="53" spans="1:13">
       <c r="A53">
         <v>46</v>
       </c>
       <c r="B53">
         <v>2</v>
       </c>
-      <c r="C53" t="s">
-        <v>201</v>
+      <c r="C53" s="7" t="s">
+        <v>194</v>
       </c>
       <c r="D53" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="E53" t="s">
+        <v>128</v>
+      </c>
+      <c r="F53" t="s">
         <v>129</v>
       </c>
-      <c r="F53" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="54" spans="1:12">
+    </row>
+    <row r="54" spans="1:13">
       <c r="A54">
         <v>47</v>
       </c>
       <c r="B54">
         <v>8</v>
       </c>
-      <c r="C54" t="s">
-        <v>202</v>
+      <c r="C54" s="7" t="s">
+        <v>195</v>
       </c>
       <c r="D54" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="E54" t="s">
+        <v>128</v>
+      </c>
+      <c r="F54" t="s">
         <v>129</v>
       </c>
-      <c r="F54" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="55" spans="1:12">
+      <c r="M54" s="6" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13">
       <c r="A55">
         <v>48</v>
       </c>
       <c r="B55">
         <v>4</v>
       </c>
-      <c r="C55" t="s">
-        <v>203</v>
+      <c r="C55" s="7" t="s">
+        <v>196</v>
       </c>
       <c r="D55" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E55" t="s">
+        <v>128</v>
+      </c>
+      <c r="F55" t="s">
         <v>129</v>
       </c>
-      <c r="F55" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="56" spans="1:12">
+    </row>
+    <row r="56" spans="1:13">
       <c r="A56" s="3">
         <v>49</v>
       </c>
       <c r="B56">
         <v>4</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C56" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="D56" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="E56" t="s">
+        <v>128</v>
+      </c>
+      <c r="F56" t="s">
+        <v>129</v>
+      </c>
+      <c r="J56" s="6" t="s">
         <v>204</v>
       </c>
-      <c r="D56" t="s">
-        <v>148</v>
-      </c>
-      <c r="E56" t="s">
-        <v>129</v>
-      </c>
-      <c r="F56" t="s">
-        <v>130</v>
-      </c>
-      <c r="J56" s="6" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="57" spans="1:12">
+    </row>
+    <row r="57" spans="1:13">
       <c r="A57" s="3">
         <v>50</v>
       </c>
       <c r="B57">
         <v>2</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C57" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="D57" t="s">
+        <v>144</v>
+      </c>
+      <c r="E57" t="s">
+        <v>128</v>
+      </c>
+      <c r="F57" t="s">
+        <v>129</v>
+      </c>
+      <c r="J57" s="6" t="s">
         <v>205</v>
       </c>
-      <c r="D57" t="s">
-        <v>149</v>
-      </c>
-      <c r="E57" t="s">
-        <v>129</v>
-      </c>
-      <c r="F57" t="s">
-        <v>130</v>
-      </c>
-      <c r="J57" s="6" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="58" spans="1:12">
+    </row>
+    <row r="58" spans="1:13">
       <c r="A58">
         <v>51</v>
       </c>
       <c r="B58">
         <v>2</v>
       </c>
-      <c r="C58" t="s">
-        <v>206</v>
+      <c r="C58" s="7" t="s">
+        <v>199</v>
       </c>
       <c r="D58" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="E58" t="s">
+        <v>128</v>
+      </c>
+      <c r="F58" t="s">
         <v>129</v>
       </c>
-      <c r="F58" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="59" spans="1:12">
+    </row>
+    <row r="59" spans="1:13">
       <c r="A59">
         <v>52</v>
       </c>
       <c r="B59">
         <v>1</v>
       </c>
-      <c r="C59" t="s">
-        <v>151</v>
+      <c r="C59" s="7" t="s">
+        <v>146</v>
       </c>
       <c r="D59" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="E59" t="s">
+        <v>128</v>
+      </c>
+      <c r="F59" t="s">
         <v>129</v>
       </c>
-      <c r="F59" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="60" spans="1:12">
+      <c r="M59" s="6" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13">
       <c r="A60">
         <v>53</v>
       </c>
       <c r="B60">
         <v>2</v>
       </c>
-      <c r="C60" t="s">
-        <v>207</v>
-      </c>
-      <c r="D60" t="s">
-        <v>153</v>
+      <c r="C60" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="D60" s="6" t="s">
+        <v>221</v>
       </c>
       <c r="E60" t="s">
+        <v>128</v>
+      </c>
+      <c r="F60" t="s">
         <v>129</v>
       </c>
-      <c r="F60" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="61" spans="1:12">
+    </row>
+    <row r="61" spans="1:13">
       <c r="A61">
         <v>54</v>
       </c>
       <c r="B61">
         <v>2</v>
       </c>
-      <c r="C61" t="s">
-        <v>208</v>
-      </c>
-      <c r="D61" t="s">
-        <v>154</v>
+      <c r="C61" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="D61" s="6" t="s">
+        <v>220</v>
       </c>
       <c r="E61" t="s">
+        <v>128</v>
+      </c>
+      <c r="F61" t="s">
         <v>129</v>
       </c>
-      <c r="F61" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="62" spans="1:12">
+    </row>
+    <row r="62" spans="1:13">
       <c r="A62">
         <v>55</v>
       </c>
@@ -2348,62 +2463,65 @@
         <v>1</v>
       </c>
       <c r="C62" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="D62" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="E62" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="F62" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="J62" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="L62">
         <v>311020047</v>
       </c>
     </row>
-    <row r="63" spans="1:12">
+    <row r="63" spans="1:13">
       <c r="A63">
         <v>56</v>
       </c>
       <c r="B63">
         <v>1</v>
       </c>
-      <c r="C63" t="s">
-        <v>160</v>
+      <c r="C63" s="7" t="s">
+        <v>153</v>
       </c>
       <c r="D63" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="E63" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="F63" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="64" spans="1:12">
+        <v>156</v>
+      </c>
+      <c r="M63" s="6" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13">
       <c r="A64" s="3">
         <v>57</v>
       </c>
       <c r="B64">
         <v>1</v>
       </c>
-      <c r="C64" t="s">
-        <v>164</v>
+      <c r="C64" s="7" t="s">
+        <v>157</v>
       </c>
       <c r="D64" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="E64" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="F64" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
     </row>
     <row r="65" spans="1:10">
@@ -2413,17 +2531,17 @@
       <c r="B65">
         <v>1</v>
       </c>
-      <c r="C65" t="s">
-        <v>168</v>
+      <c r="C65" s="7" t="s">
+        <v>161</v>
       </c>
       <c r="D65" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="E65" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="F65" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
     </row>
     <row r="66" spans="1:10">
@@ -2433,20 +2551,20 @@
       <c r="B66">
         <v>1</v>
       </c>
-      <c r="C66" t="s">
-        <v>172</v>
+      <c r="C66" s="7" t="s">
+        <v>165</v>
       </c>
       <c r="D66" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="E66" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="F66" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="J66" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
     </row>
     <row r="67" spans="1:10">
@@ -2457,16 +2575,16 @@
         <v>1</v>
       </c>
       <c r="C67" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="D67" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="E67" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="F67" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
     </row>
     <row r="68" spans="1:10">
@@ -2476,17 +2594,17 @@
       <c r="B68">
         <v>1</v>
       </c>
-      <c r="C68" t="s">
-        <v>181</v>
+      <c r="C68" s="7" t="s">
+        <v>174</v>
       </c>
       <c r="D68" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="E68" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="F68" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
     </row>
     <row r="69" spans="1:10">
@@ -2496,33 +2614,33 @@
       <c r="B69">
         <v>1</v>
       </c>
-      <c r="C69" t="s">
-        <v>185</v>
+      <c r="C69" s="7" t="s">
+        <v>178</v>
       </c>
       <c r="D69" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="E69" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="F69" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="J69" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
     </row>
     <row r="70" spans="1:10" ht="30">
       <c r="J70" s="4" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
     </row>
     <row r="73" spans="1:10" ht="30">
       <c r="D73" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="J73" s="4" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
various annotations and changes
</commit_message>
<xml_diff>
--- a/Nestbox_v2/BOM_Nestbox_v2.xlsx
+++ b/Nestbox_v2/BOM_Nestbox_v2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3000" windowWidth="30160" windowHeight="23540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="BOM_Nestbox_v2.csv" sheetId="1" r:id="rId1"/>
@@ -755,7 +755,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -792,6 +792,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -802,7 +814,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="26">
+  <cellStyleXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -829,8 +841,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -841,8 +861,10 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="26">
+  <cellStyles count="34">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -857,6 +879,10 @@
     <cellStyle name="Followed Hyperlink" xfId="21" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="23" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="25" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="27" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="29" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="31" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="33" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -868,6 +894,10 @@
     <cellStyle name="Hyperlink" xfId="20" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="22" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="24" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="26" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="28" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="30" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="32" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1199,14 +1229,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A56" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="D64" sqref="D64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="3" max="3" width="44" customWidth="1"/>
     <col min="4" max="4" width="23.6640625" customWidth="1"/>
+    <col min="7" max="9" width="0" hidden="1" customWidth="1"/>
+    <col min="10" max="11" width="10.83203125" hidden="1" customWidth="1"/>
     <col min="13" max="13" width="10.83203125" style="6"/>
   </cols>
   <sheetData>
@@ -1415,7 +1447,7 @@
       </c>
     </row>
     <row r="14" spans="1:13">
-      <c r="A14">
+      <c r="A14" s="8">
         <v>7</v>
       </c>
       <c r="B14">
@@ -2482,7 +2514,7 @@
       </c>
     </row>
     <row r="63" spans="1:13">
-      <c r="A63">
+      <c r="A63" s="9">
         <v>56</v>
       </c>
       <c r="B63">

</xml_diff>